<commit_message>
Updating project list and export files
</commit_message>
<xml_diff>
--- a/raw/project_Zooscan_standardizer.xlsx
+++ b/raw/project_Zooscan_standardizer.xlsx
@@ -19085,20 +19085,20 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Variables</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Variable_types</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
@@ -19870,6 +19870,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating step 0 to remove project with revoked access rights and step 2 to start by updating taxonomic annotations and include the column ROI_number in the standardized files
</commit_message>
<xml_diff>
--- a/raw/project_Zooscan_standardizer.xlsx
+++ b/raw/project_Zooscan_standardizer.xlsx
@@ -510,7 +510,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AS92"/>
+  <dimension ref="A1:AS91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16031,11 +16031,11 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>5785</v>
+        <v>5930</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>https://ecotaxa.obs-vlfr.fr/prj/5785</t>
+          <t>https://ecotaxa.obs-vlfr.fr/prj/5930</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -16194,13 +16194,11 @@
       </c>
       <c r="AK78" t="inlineStr">
         <is>
-          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_5785_flags.csv</t>
-        </is>
-      </c>
-      <c r="AL78" t="inlineStr">
-        <is>
-          <t>99999;nan</t>
-        </is>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_5930_flags.csv</t>
+        </is>
+      </c>
+      <c r="AL78" t="n">
+        <v>999999</v>
       </c>
       <c r="AM78" t="inlineStr"/>
       <c r="AN78" t="inlineStr">
@@ -16236,11 +16234,11 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>5930</v>
+        <v>6044</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://ecotaxa.obs-vlfr.fr/prj/5930</t>
+          <t>https://ecotaxa.obs-vlfr.fr/prj/6044</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -16399,7 +16397,7 @@
       </c>
       <c r="AK79" t="inlineStr">
         <is>
-          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_5930_flags.csv</t>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6044_flags.csv</t>
         </is>
       </c>
       <c r="AL79" t="n">
@@ -16439,11 +16437,11 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>6044</v>
+        <v>6048</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://ecotaxa.obs-vlfr.fr/prj/6044</t>
+          <t>https://ecotaxa.obs-vlfr.fr/prj/6048</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -16602,7 +16600,7 @@
       </c>
       <c r="AK80" t="inlineStr">
         <is>
-          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6044_flags.csv</t>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6048_flags.csv</t>
         </is>
       </c>
       <c r="AL80" t="n">
@@ -16642,11 +16640,11 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>6048</v>
+        <v>6111</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://ecotaxa.obs-vlfr.fr/prj/6048</t>
+          <t>https://ecotaxa.obs-vlfr.fr/prj/6111</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -16805,7 +16803,7 @@
       </c>
       <c r="AK81" t="inlineStr">
         <is>
-          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6048_flags.csv</t>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6111_flags.csv</t>
         </is>
       </c>
       <c r="AL81" t="n">
@@ -16845,11 +16843,11 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>6111</v>
+        <v>6262</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://ecotaxa.obs-vlfr.fr/prj/6111</t>
+          <t>https://ecotaxa.obs-vlfr.fr/prj/6262</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -17008,7 +17006,7 @@
       </c>
       <c r="AK82" t="inlineStr">
         <is>
-          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6111_flags.csv</t>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6262_flags.csv</t>
         </is>
       </c>
       <c r="AL82" t="n">
@@ -17048,11 +17046,11 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>6262</v>
+        <v>6270</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>https://ecotaxa.obs-vlfr.fr/prj/6262</t>
+          <t>https://ecotaxa.obs-vlfr.fr/prj/6270</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -17211,7 +17209,7 @@
       </c>
       <c r="AK83" t="inlineStr">
         <is>
-          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6262_flags.csv</t>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6270_flags.csv</t>
         </is>
       </c>
       <c r="AL83" t="n">
@@ -17251,11 +17249,11 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>6270</v>
+        <v>6280</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>https://ecotaxa.obs-vlfr.fr/prj/6270</t>
+          <t>https://ecotaxa.obs-vlfr.fr/prj/6280</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -17414,7 +17412,7 @@
       </c>
       <c r="AK84" t="inlineStr">
         <is>
-          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6270_flags.csv</t>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6280_flags.csv</t>
         </is>
       </c>
       <c r="AL84" t="n">
@@ -17454,11 +17452,11 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>6280</v>
+        <v>6307</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>https://ecotaxa.obs-vlfr.fr/prj/6280</t>
+          <t>https://ecotaxa.obs-vlfr.fr/prj/6307</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -17617,7 +17615,7 @@
       </c>
       <c r="AK85" t="inlineStr">
         <is>
-          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6280_flags.csv</t>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6307_flags.csv</t>
         </is>
       </c>
       <c r="AL85" t="n">
@@ -17657,11 +17655,11 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>6307</v>
+        <v>6341</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>https://ecotaxa.obs-vlfr.fr/prj/6307</t>
+          <t>https://ecotaxa.obs-vlfr.fr/prj/6341</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -17820,7 +17818,7 @@
       </c>
       <c r="AK86" t="inlineStr">
         <is>
-          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6307_flags.csv</t>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6341_flags.csv</t>
         </is>
       </c>
       <c r="AL86" t="n">
@@ -17860,11 +17858,11 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>6341</v>
+        <v>6342</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>https://ecotaxa.obs-vlfr.fr/prj/6341</t>
+          <t>https://ecotaxa.obs-vlfr.fr/prj/6342</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -18023,7 +18021,7 @@
       </c>
       <c r="AK87" t="inlineStr">
         <is>
-          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6341_flags.csv</t>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6342_flags.csv</t>
         </is>
       </c>
       <c r="AL87" t="n">
@@ -18063,11 +18061,11 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>6342</v>
+        <v>6343</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>https://ecotaxa.obs-vlfr.fr/prj/6342</t>
+          <t>https://ecotaxa.obs-vlfr.fr/prj/6343</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -18226,7 +18224,7 @@
       </c>
       <c r="AK88" t="inlineStr">
         <is>
-          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6342_flags.csv</t>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6343_flags.csv</t>
         </is>
       </c>
       <c r="AL88" t="n">
@@ -18266,11 +18264,11 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>6343</v>
+        <v>6358</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>https://ecotaxa.obs-vlfr.fr/prj/6343</t>
+          <t>https://ecotaxa.obs-vlfr.fr/prj/6358</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -18429,7 +18427,7 @@
       </c>
       <c r="AK89" t="inlineStr">
         <is>
-          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6343_flags.csv</t>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6358_flags.csv</t>
         </is>
       </c>
       <c r="AL89" t="n">
@@ -18469,11 +18467,11 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>6358</v>
+        <v>6579</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>https://ecotaxa.obs-vlfr.fr/prj/6358</t>
+          <t>https://ecotaxa.obs-vlfr.fr/prj/6579</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -18491,16 +18489,8 @@
           <t>sample_program</t>
         </is>
       </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>sample_stationid</t>
-        </is>
-      </c>
-      <c r="G90" t="inlineStr">
-        <is>
-          <t>sample_tow_nb</t>
-        </is>
-      </c>
+      <c r="F90" t="inlineStr"/>
+      <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
         <is>
           <t>sample_id</t>
@@ -18632,7 +18622,7 @@
       </c>
       <c r="AK90" t="inlineStr">
         <is>
-          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6358_flags.csv</t>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6579_flags.csv</t>
         </is>
       </c>
       <c r="AL90" t="n">
@@ -18672,11 +18662,11 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>6579</v>
+        <v>6729</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>https://ecotaxa.obs-vlfr.fr/prj/6579</t>
+          <t>https://ecotaxa.obs-vlfr.fr/prj/6729</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -18694,8 +18684,16 @@
           <t>sample_program</t>
         </is>
       </c>
-      <c r="F91" t="inlineStr"/>
-      <c r="G91" t="inlineStr"/>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>sample_stationid</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>sample_tow_nb</t>
+        </is>
+      </c>
       <c r="H91" t="inlineStr">
         <is>
           <t>sample_id</t>
@@ -18827,7 +18825,7 @@
       </c>
       <c r="AK91" t="inlineStr">
         <is>
-          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6579_flags.csv</t>
+          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6729_flags.csv</t>
         </is>
       </c>
       <c r="AL91" t="n">
@@ -18860,209 +18858,6 @@
         </is>
       </c>
       <c r="AS91" t="inlineStr">
-        <is>
-          <t>net_mesh:{field:sample_net_mesh,unit:micrometer};net_aperture:{field:sample_net_surf,unit:square_meter}</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="n">
-        <v>6729</v>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>https://ecotaxa.obs-vlfr.fr/prj/6729</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>~/GIT/PSSdb/raw/ecotaxa</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>Zooscan</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>sample_program</t>
-        </is>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>sample_stationid</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>sample_tow_nb</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>sample_id</t>
-        </is>
-      </c>
-      <c r="I92" t="inlineStr">
-        <is>
-          <t>object_lat</t>
-        </is>
-      </c>
-      <c r="J92" t="inlineStr">
-        <is>
-          <t>degree</t>
-        </is>
-      </c>
-      <c r="K92" t="inlineStr">
-        <is>
-          <t>object_lon</t>
-        </is>
-      </c>
-      <c r="L92" t="inlineStr">
-        <is>
-          <t>degree</t>
-        </is>
-      </c>
-      <c r="M92" t="inlineStr">
-        <is>
-          <t>object_depth_min</t>
-        </is>
-      </c>
-      <c r="N92" t="inlineStr">
-        <is>
-          <t>meter</t>
-        </is>
-      </c>
-      <c r="O92" t="inlineStr">
-        <is>
-          <t>object_depth_max</t>
-        </is>
-      </c>
-      <c r="P92" t="inlineStr">
-        <is>
-          <t>meter</t>
-        </is>
-      </c>
-      <c r="Q92" t="inlineStr">
-        <is>
-          <t>object_date</t>
-        </is>
-      </c>
-      <c r="R92" t="inlineStr">
-        <is>
-          <t>%Y%m%d</t>
-        </is>
-      </c>
-      <c r="S92" t="inlineStr">
-        <is>
-          <t>object_time</t>
-        </is>
-      </c>
-      <c r="T92" t="inlineStr">
-        <is>
-          <t>%H%M%S</t>
-        </is>
-      </c>
-      <c r="U92" t="inlineStr">
-        <is>
-          <t>sample_tot_vol</t>
-        </is>
-      </c>
-      <c r="V92" t="inlineStr">
-        <is>
-          <t>cubic_meter</t>
-        </is>
-      </c>
-      <c r="W92" t="inlineStr">
-        <is>
-          <t>acq_sub_part</t>
-        </is>
-      </c>
-      <c r="X92" t="inlineStr">
-        <is>
-          <t>object_id</t>
-        </is>
-      </c>
-      <c r="Y92" t="inlineStr"/>
-      <c r="Z92" t="inlineStr"/>
-      <c r="AA92" t="inlineStr"/>
-      <c r="AB92" t="inlineStr"/>
-      <c r="AC92" t="inlineStr">
-        <is>
-          <t>object_area</t>
-        </is>
-      </c>
-      <c r="AD92" t="inlineStr">
-        <is>
-          <t>square_pixel</t>
-        </is>
-      </c>
-      <c r="AE92" t="inlineStr">
-        <is>
-          <t>object_minor</t>
-        </is>
-      </c>
-      <c r="AF92" t="inlineStr">
-        <is>
-          <t>pixel</t>
-        </is>
-      </c>
-      <c r="AG92" t="inlineStr">
-        <is>
-          <t>process_particle_pixel_size_mm</t>
-        </is>
-      </c>
-      <c r="AH92" t="inlineStr">
-        <is>
-          <t>millimeter_per_pixel</t>
-        </is>
-      </c>
-      <c r="AI92" t="inlineStr">
-        <is>
-          <t>object_annotation_category</t>
-        </is>
-      </c>
-      <c r="AJ92" t="inlineStr">
-        <is>
-          <t>object_annotation_status</t>
-        </is>
-      </c>
-      <c r="AK92" t="inlineStr">
-        <is>
-          <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_6729_flags.csv</t>
-        </is>
-      </c>
-      <c r="AL92" t="n">
-        <v>999999</v>
-      </c>
-      <c r="AM92" t="inlineStr"/>
-      <c r="AN92" t="inlineStr">
-        <is>
-          <t>sample_net_type</t>
-        </is>
-      </c>
-      <c r="AO92" t="inlineStr">
-        <is>
-          <t>acq_min_mesh</t>
-        </is>
-      </c>
-      <c r="AP92" t="inlineStr">
-        <is>
-          <t>micrometer</t>
-        </is>
-      </c>
-      <c r="AQ92" t="inlineStr">
-        <is>
-          <t>acq_max_mesh</t>
-        </is>
-      </c>
-      <c r="AR92" t="inlineStr">
-        <is>
-          <t>micrometer</t>
-        </is>
-      </c>
-      <c r="AS92" t="inlineStr">
         <is>
           <t>net_mesh:{field:sample_net_mesh,unit:micrometer};net_aperture:{field:sample_net_surf,unit:square_meter}</t>
         </is>

</xml_diff>

<commit_message>
Upating nbss regression with log-transformation
</commit_message>
<xml_diff>
--- a/raw/project_Zooscan_standardizer.xlsx
+++ b/raw/project_Zooscan_standardizer.xlsx
@@ -8,15 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dugennem/GIT/PSSdb/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A83DEC-36F1-0547-9468-D54FF4D571E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EC3339-1F99-0248-BA31-97B88B1154A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1014,6 +1027,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -1027,6 +1041,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1430,9 +1445,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AU93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B93" sqref="B93"/>
+      <selection pane="bottomLeft" activeCell="AJ92" sqref="AJ92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updating project list and including new instruments - Planktoscope and FlowCam-
</commit_message>
<xml_diff>
--- a/raw/project_Zooscan_standardizer.xlsx
+++ b/raw/project_Zooscan_standardizer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dugennem/GIT/PSSdb/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00EC3339-1F99-0248-BA31-97B88B1154A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4C926B-AA81-424F-88BB-DC25943AF523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,25 +16,12 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3835" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3754" uniqueCount="320">
   <si>
     <t>Project_ID</t>
   </si>
@@ -681,15 +668,6 @@
     <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_3166_flags.csv</t>
   </si>
   <si>
-    <t>https://ecotaxa.obs-vlfr.fr/prj/3274</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_3274_flags.csv</t>
-  </si>
-  <si>
-    <t>999;99999;999999</t>
-  </si>
-  <si>
     <t>https://ecotaxa.obs-vlfr.fr/prj/3391</t>
   </si>
   <si>
@@ -724,12 +702,6 @@
   </si>
   <si>
     <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_4025_flags.csv</t>
-  </si>
-  <si>
-    <t>https://ecotaxa.obs-vlfr.fr/prj/4172</t>
-  </si>
-  <si>
-    <t>~/GIT/PSSdb/raw/flags/ecotaxa/project_4172_flags.csv</t>
   </si>
   <si>
     <t>https://ecotaxa.obs-vlfr.fr/prj/4429</t>
@@ -1015,24 +987,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1052,7 +1010,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1075,38 +1033,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1443,203 +1380,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AU93"/>
+  <dimension ref="A1:AU91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ92" sqref="AJ92"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65:XFD65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="23" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="17" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="25" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="22" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="85.33203125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="3" t="s">
+      <c r="AL1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AM1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AN1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AO1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="3" t="s">
+      <c r="AP1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="3" t="s">
+      <c r="AR1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="3" t="s">
+      <c r="AS1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="3" t="s">
+      <c r="AT1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="3" t="s">
+      <c r="AU1" s="1" t="s">
         <v>46</v>
       </c>
     </row>
@@ -9694,7 +9582,7 @@
     </row>
     <row r="65" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>3274</v>
+        <v>3391</v>
       </c>
       <c r="B65" t="s">
         <v>215</v>
@@ -9805,10 +9693,10 @@
         <v>78</v>
       </c>
       <c r="AQ65" t="s">
-        <v>185</v>
+        <v>79</v>
       </c>
       <c r="AR65" t="s">
-        <v>186</v>
+        <v>80</v>
       </c>
       <c r="AS65" t="s">
         <v>81</v>
@@ -9822,7 +9710,7 @@
     </row>
     <row r="66" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>3391</v>
+        <v>3607</v>
       </c>
       <c r="B66" t="s">
         <v>218</v>
@@ -9926,11 +9814,8 @@
       <c r="AM66" t="s">
         <v>219</v>
       </c>
-      <c r="AN66" t="s">
-        <v>220</v>
-      </c>
-      <c r="AP66" t="s">
-        <v>78</v>
+      <c r="AN66">
+        <v>999999</v>
       </c>
       <c r="AQ66" t="s">
         <v>79</v>
@@ -9950,10 +9835,10 @@
     </row>
     <row r="67" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>3607</v>
+        <v>3657</v>
       </c>
       <c r="B67" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C67" t="s">
         <v>48</v>
@@ -10052,11 +9937,14 @@
         <v>76</v>
       </c>
       <c r="AM67" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AN67">
         <v>999999</v>
       </c>
+      <c r="AP67" t="s">
+        <v>78</v>
+      </c>
       <c r="AQ67" t="s">
         <v>79</v>
       </c>
@@ -10075,10 +9963,10 @@
     </row>
     <row r="68" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>3657</v>
+        <v>4023</v>
       </c>
       <c r="B68" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C68" t="s">
         <v>48</v>
@@ -10086,127 +9974,13 @@
       <c r="D68" t="s">
         <v>49</v>
       </c>
-      <c r="E68" t="s">
-        <v>50</v>
-      </c>
-      <c r="F68" t="s">
-        <v>51</v>
-      </c>
-      <c r="G68" t="s">
-        <v>52</v>
-      </c>
-      <c r="H68" t="s">
-        <v>53</v>
-      </c>
-      <c r="I68" t="s">
-        <v>54</v>
-      </c>
-      <c r="J68" t="s">
-        <v>55</v>
-      </c>
-      <c r="K68" t="s">
-        <v>56</v>
-      </c>
-      <c r="L68" t="s">
-        <v>55</v>
-      </c>
-      <c r="M68" t="s">
-        <v>57</v>
-      </c>
-      <c r="N68" t="s">
-        <v>58</v>
-      </c>
-      <c r="O68" t="s">
-        <v>59</v>
-      </c>
-      <c r="P68" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q68" t="s">
-        <v>60</v>
-      </c>
-      <c r="R68" t="s">
-        <v>61</v>
-      </c>
-      <c r="S68" t="s">
-        <v>62</v>
-      </c>
-      <c r="T68" t="s">
-        <v>63</v>
-      </c>
-      <c r="U68" t="s">
-        <v>64</v>
-      </c>
-      <c r="V68" t="s">
-        <v>65</v>
-      </c>
-      <c r="W68" t="s">
-        <v>66</v>
-      </c>
-      <c r="X68" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC68" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD68" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE68" t="s">
-        <v>70</v>
-      </c>
-      <c r="AF68" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG68" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH68" t="s">
-        <v>71</v>
-      </c>
-      <c r="AI68" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ68" t="s">
-        <v>74</v>
-      </c>
-      <c r="AK68" t="s">
-        <v>75</v>
-      </c>
-      <c r="AL68" t="s">
-        <v>76</v>
-      </c>
-      <c r="AM68" t="s">
-        <v>224</v>
-      </c>
-      <c r="AN68">
-        <v>999999</v>
-      </c>
-      <c r="AP68" t="s">
-        <v>78</v>
-      </c>
-      <c r="AQ68" t="s">
-        <v>79</v>
-      </c>
-      <c r="AR68" t="s">
-        <v>80</v>
-      </c>
-      <c r="AS68" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT68" t="s">
-        <v>80</v>
-      </c>
-      <c r="AU68" t="s">
-        <v>82</v>
-      </c>
     </row>
     <row r="69" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>4023</v>
+        <v>4024</v>
       </c>
       <c r="B69" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C69" t="s">
         <v>48</v>
@@ -10214,13 +9988,127 @@
       <c r="D69" t="s">
         <v>49</v>
       </c>
+      <c r="E69" t="s">
+        <v>50</v>
+      </c>
+      <c r="F69" t="s">
+        <v>51</v>
+      </c>
+      <c r="G69" t="s">
+        <v>52</v>
+      </c>
+      <c r="H69" t="s">
+        <v>53</v>
+      </c>
+      <c r="I69" t="s">
+        <v>54</v>
+      </c>
+      <c r="J69" t="s">
+        <v>55</v>
+      </c>
+      <c r="K69" t="s">
+        <v>56</v>
+      </c>
+      <c r="L69" t="s">
+        <v>55</v>
+      </c>
+      <c r="M69" t="s">
+        <v>57</v>
+      </c>
+      <c r="N69" t="s">
+        <v>58</v>
+      </c>
+      <c r="O69" t="s">
+        <v>59</v>
+      </c>
+      <c r="P69" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>60</v>
+      </c>
+      <c r="R69" t="s">
+        <v>61</v>
+      </c>
+      <c r="S69" t="s">
+        <v>62</v>
+      </c>
+      <c r="T69" t="s">
+        <v>63</v>
+      </c>
+      <c r="U69" t="s">
+        <v>64</v>
+      </c>
+      <c r="V69" t="s">
+        <v>65</v>
+      </c>
+      <c r="W69" t="s">
+        <v>66</v>
+      </c>
+      <c r="X69" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC69" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD69" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE69" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF69" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG69" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH69" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI69" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ69" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK69" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL69" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM69" t="s">
+        <v>224</v>
+      </c>
+      <c r="AN69">
+        <v>999999</v>
+      </c>
+      <c r="AP69" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ69" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR69" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS69" t="s">
+        <v>81</v>
+      </c>
+      <c r="AT69" t="s">
+        <v>80</v>
+      </c>
+      <c r="AU69" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="70" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>4024</v>
+        <v>4025</v>
       </c>
       <c r="B70" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C70" t="s">
         <v>48</v>
@@ -10319,7 +10207,7 @@
         <v>76</v>
       </c>
       <c r="AM70" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="AN70">
         <v>999999</v>
@@ -10345,10 +10233,10 @@
     </row>
     <row r="71" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>4025</v>
+        <v>4429</v>
       </c>
       <c r="B71" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C71" t="s">
         <v>48</v>
@@ -10447,7 +10335,7 @@
         <v>76</v>
       </c>
       <c r="AM71" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AN71">
         <v>999999</v>
@@ -10473,10 +10361,10 @@
     </row>
     <row r="72" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>4172</v>
+        <v>4533</v>
       </c>
       <c r="B72" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C72" t="s">
         <v>48</v>
@@ -10575,7 +10463,7 @@
         <v>76</v>
       </c>
       <c r="AM72" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AN72">
         <v>999999</v>
@@ -10601,10 +10489,10 @@
     </row>
     <row r="73" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>4429</v>
+        <v>4534</v>
       </c>
       <c r="B73" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C73" t="s">
         <v>48</v>
@@ -10703,7 +10591,7 @@
         <v>76</v>
       </c>
       <c r="AM73" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AN73">
         <v>999999</v>
@@ -10729,10 +10617,10 @@
     </row>
     <row r="74" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>4533</v>
+        <v>4598</v>
       </c>
       <c r="B74" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C74" t="s">
         <v>48</v>
@@ -10831,7 +10719,7 @@
         <v>76</v>
       </c>
       <c r="AM74" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="AN74">
         <v>999999</v>
@@ -10857,10 +10745,10 @@
     </row>
     <row r="75" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>4534</v>
+        <v>4904</v>
       </c>
       <c r="B75" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C75" t="s">
         <v>48</v>
@@ -10959,10 +10847,10 @@
         <v>76</v>
       </c>
       <c r="AM75" t="s">
-        <v>237</v>
-      </c>
-      <c r="AN75">
-        <v>999999</v>
+        <v>236</v>
+      </c>
+      <c r="AN75" t="s">
+        <v>217</v>
       </c>
       <c r="AP75" t="s">
         <v>78</v>
@@ -10985,10 +10873,10 @@
     </row>
     <row r="76" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>4598</v>
+        <v>5930</v>
       </c>
       <c r="B76" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C76" t="s">
         <v>48</v>
@@ -11087,7 +10975,7 @@
         <v>76</v>
       </c>
       <c r="AM76" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AN76">
         <v>999999</v>
@@ -11113,10 +11001,10 @@
     </row>
     <row r="77" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>4904</v>
+        <v>6048</v>
       </c>
       <c r="B77" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C77" t="s">
         <v>48</v>
@@ -11215,10 +11103,10 @@
         <v>76</v>
       </c>
       <c r="AM77" t="s">
-        <v>241</v>
-      </c>
-      <c r="AN77" t="s">
-        <v>220</v>
+        <v>240</v>
+      </c>
+      <c r="AN77">
+        <v>999999</v>
       </c>
       <c r="AP77" t="s">
         <v>78</v>
@@ -11241,10 +11129,10 @@
     </row>
     <row r="78" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>5930</v>
+        <v>6111</v>
       </c>
       <c r="B78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C78" t="s">
         <v>48</v>
@@ -11343,7 +11231,7 @@
         <v>76</v>
       </c>
       <c r="AM78" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="AN78">
         <v>999999</v>
@@ -11369,10 +11257,10 @@
     </row>
     <row r="79" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>6048</v>
+        <v>6262</v>
       </c>
       <c r="B79" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C79" t="s">
         <v>48</v>
@@ -11471,7 +11359,7 @@
         <v>76</v>
       </c>
       <c r="AM79" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AN79">
         <v>999999</v>
@@ -11497,10 +11385,10 @@
     </row>
     <row r="80" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>6111</v>
+        <v>6270</v>
       </c>
       <c r="B80" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C80" t="s">
         <v>48</v>
@@ -11599,7 +11487,7 @@
         <v>76</v>
       </c>
       <c r="AM80" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AN80">
         <v>999999</v>
@@ -11625,10 +11513,10 @@
     </row>
     <row r="81" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>6262</v>
+        <v>6280</v>
       </c>
       <c r="B81" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C81" t="s">
         <v>48</v>
@@ -11727,7 +11615,7 @@
         <v>76</v>
       </c>
       <c r="AM81" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AN81">
         <v>999999</v>
@@ -11753,10 +11641,10 @@
     </row>
     <row r="82" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>6270</v>
+        <v>6307</v>
       </c>
       <c r="B82" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C82" t="s">
         <v>48</v>
@@ -11855,7 +11743,7 @@
         <v>76</v>
       </c>
       <c r="AM82" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AN82">
         <v>999999</v>
@@ -11881,10 +11769,10 @@
     </row>
     <row r="83" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>6280</v>
+        <v>6341</v>
       </c>
       <c r="B83" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C83" t="s">
         <v>48</v>
@@ -11983,7 +11871,7 @@
         <v>76</v>
       </c>
       <c r="AM83" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AN83">
         <v>999999</v>
@@ -12009,10 +11897,10 @@
     </row>
     <row r="84" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>6307</v>
+        <v>6342</v>
       </c>
       <c r="B84" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C84" t="s">
         <v>48</v>
@@ -12111,7 +11999,7 @@
         <v>76</v>
       </c>
       <c r="AM84" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AN84">
         <v>999999</v>
@@ -12137,10 +12025,10 @@
     </row>
     <row r="85" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>6341</v>
+        <v>6343</v>
       </c>
       <c r="B85" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C85" t="s">
         <v>48</v>
@@ -12239,7 +12127,7 @@
         <v>76</v>
       </c>
       <c r="AM85" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AN85">
         <v>999999</v>
@@ -12265,10 +12153,10 @@
     </row>
     <row r="86" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>6342</v>
+        <v>6358</v>
       </c>
       <c r="B86" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C86" t="s">
         <v>48</v>
@@ -12367,7 +12255,7 @@
         <v>76</v>
       </c>
       <c r="AM86" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AN86">
         <v>999999</v>
@@ -12393,10 +12281,10 @@
     </row>
     <row r="87" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>6343</v>
+        <v>6579</v>
       </c>
       <c r="B87" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C87" t="s">
         <v>48</v>
@@ -12407,12 +12295,6 @@
       <c r="E87" t="s">
         <v>50</v>
       </c>
-      <c r="F87" t="s">
-        <v>51</v>
-      </c>
-      <c r="G87" t="s">
-        <v>52</v>
-      </c>
       <c r="H87" t="s">
         <v>53</v>
       </c>
@@ -12495,7 +12377,7 @@
         <v>76</v>
       </c>
       <c r="AM87" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AN87">
         <v>999999</v>
@@ -12521,10 +12403,10 @@
     </row>
     <row r="88" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>6358</v>
+        <v>6212</v>
       </c>
       <c r="B88" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C88" t="s">
         <v>48</v>
@@ -12623,7 +12505,7 @@
         <v>76</v>
       </c>
       <c r="AM88" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="AN88">
         <v>999999</v>
@@ -12649,10 +12531,10 @@
     </row>
     <row r="89" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>6579</v>
+        <v>8788</v>
       </c>
       <c r="B89" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C89" t="s">
         <v>48</v>
@@ -12663,6 +12545,12 @@
       <c r="E89" t="s">
         <v>50</v>
       </c>
+      <c r="F89" t="s">
+        <v>51</v>
+      </c>
+      <c r="G89" t="s">
+        <v>52</v>
+      </c>
       <c r="H89" t="s">
         <v>53</v>
       </c>
@@ -12745,10 +12633,10 @@
         <v>76</v>
       </c>
       <c r="AM89" t="s">
-        <v>265</v>
-      </c>
-      <c r="AN89">
-        <v>999999</v>
+        <v>264</v>
+      </c>
+      <c r="AN89" t="s">
+        <v>217</v>
       </c>
       <c r="AP89" t="s">
         <v>78</v>
@@ -12771,10 +12659,10 @@
     </row>
     <row r="90" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>6212</v>
+        <v>112</v>
       </c>
       <c r="B90" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C90" t="s">
         <v>48</v>
@@ -12861,10 +12749,10 @@
         <v>71</v>
       </c>
       <c r="AI90" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="AJ90" t="s">
-        <v>74</v>
+        <v>266</v>
       </c>
       <c r="AK90" t="s">
         <v>75</v>
@@ -12875,9 +12763,6 @@
       <c r="AM90" t="s">
         <v>267</v>
       </c>
-      <c r="AN90">
-        <v>999999</v>
-      </c>
       <c r="AP90" t="s">
         <v>78</v>
       </c>
@@ -12899,7 +12784,7 @@
     </row>
     <row r="91" spans="1:47" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>8788</v>
+        <v>113</v>
       </c>
       <c r="B91" t="s">
         <v>268</v>
@@ -13000,12 +12885,6 @@
       <c r="AL91" t="s">
         <v>76</v>
       </c>
-      <c r="AM91" t="s">
-        <v>269</v>
-      </c>
-      <c r="AN91" t="s">
-        <v>220</v>
-      </c>
       <c r="AP91" t="s">
         <v>78</v>
       </c>
@@ -13025,257 +12904,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="92" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A92">
-        <v>112</v>
-      </c>
-      <c r="B92" t="s">
-        <v>270</v>
-      </c>
-      <c r="C92" t="s">
-        <v>48</v>
-      </c>
-      <c r="D92" t="s">
-        <v>49</v>
-      </c>
-      <c r="E92" t="s">
-        <v>50</v>
-      </c>
-      <c r="F92" t="s">
-        <v>51</v>
-      </c>
-      <c r="G92" t="s">
-        <v>52</v>
-      </c>
-      <c r="H92" t="s">
-        <v>53</v>
-      </c>
-      <c r="I92" t="s">
-        <v>54</v>
-      </c>
-      <c r="J92" t="s">
-        <v>55</v>
-      </c>
-      <c r="K92" t="s">
-        <v>56</v>
-      </c>
-      <c r="L92" t="s">
-        <v>55</v>
-      </c>
-      <c r="M92" t="s">
-        <v>57</v>
-      </c>
-      <c r="N92" t="s">
-        <v>58</v>
-      </c>
-      <c r="O92" t="s">
-        <v>59</v>
-      </c>
-      <c r="P92" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q92" t="s">
-        <v>60</v>
-      </c>
-      <c r="R92" t="s">
-        <v>61</v>
-      </c>
-      <c r="S92" t="s">
-        <v>62</v>
-      </c>
-      <c r="T92" t="s">
-        <v>63</v>
-      </c>
-      <c r="U92" t="s">
-        <v>64</v>
-      </c>
-      <c r="V92" t="s">
-        <v>65</v>
-      </c>
-      <c r="W92" t="s">
-        <v>66</v>
-      </c>
-      <c r="X92" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC92" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD92" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE92" t="s">
-        <v>70</v>
-      </c>
-      <c r="AF92" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG92" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH92" t="s">
-        <v>71</v>
-      </c>
-      <c r="AI92" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ92" t="s">
-        <v>271</v>
-      </c>
-      <c r="AK92" t="s">
-        <v>75</v>
-      </c>
-      <c r="AL92" t="s">
-        <v>76</v>
-      </c>
-      <c r="AM92" t="s">
-        <v>272</v>
-      </c>
-      <c r="AP92" t="s">
-        <v>78</v>
-      </c>
-      <c r="AQ92" t="s">
-        <v>79</v>
-      </c>
-      <c r="AR92" t="s">
-        <v>80</v>
-      </c>
-      <c r="AS92" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT92" t="s">
-        <v>80</v>
-      </c>
-      <c r="AU92" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="93" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A93">
-        <v>113</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="C93" t="s">
-        <v>48</v>
-      </c>
-      <c r="D93" t="s">
-        <v>49</v>
-      </c>
-      <c r="E93" t="s">
-        <v>50</v>
-      </c>
-      <c r="F93" t="s">
-        <v>51</v>
-      </c>
-      <c r="G93" t="s">
-        <v>52</v>
-      </c>
-      <c r="H93" t="s">
-        <v>53</v>
-      </c>
-      <c r="I93" t="s">
-        <v>54</v>
-      </c>
-      <c r="J93" t="s">
-        <v>55</v>
-      </c>
-      <c r="K93" t="s">
-        <v>56</v>
-      </c>
-      <c r="L93" t="s">
-        <v>55</v>
-      </c>
-      <c r="M93" t="s">
-        <v>57</v>
-      </c>
-      <c r="N93" t="s">
-        <v>58</v>
-      </c>
-      <c r="O93" t="s">
-        <v>59</v>
-      </c>
-      <c r="P93" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q93" t="s">
-        <v>60</v>
-      </c>
-      <c r="R93" t="s">
-        <v>61</v>
-      </c>
-      <c r="S93" t="s">
-        <v>62</v>
-      </c>
-      <c r="T93" t="s">
-        <v>63</v>
-      </c>
-      <c r="U93" t="s">
-        <v>64</v>
-      </c>
-      <c r="V93" t="s">
-        <v>65</v>
-      </c>
-      <c r="W93" t="s">
-        <v>66</v>
-      </c>
-      <c r="X93" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC93" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD93" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE93" t="s">
-        <v>70</v>
-      </c>
-      <c r="AF93" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG93" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH93" t="s">
-        <v>71</v>
-      </c>
-      <c r="AI93" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ93" t="s">
-        <v>74</v>
-      </c>
-      <c r="AK93" t="s">
-        <v>75</v>
-      </c>
-      <c r="AL93" t="s">
-        <v>76</v>
-      </c>
-      <c r="AP93" t="s">
-        <v>78</v>
-      </c>
-      <c r="AQ93" t="s">
-        <v>79</v>
-      </c>
-      <c r="AR93" t="s">
-        <v>80</v>
-      </c>
-      <c r="AS93" t="s">
-        <v>81</v>
-      </c>
-      <c r="AT93" t="s">
-        <v>80</v>
-      </c>
-      <c r="AU93" t="s">
-        <v>82</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B93" r:id="rId1" xr:uid="{9EFF96BC-A35E-4B4D-81B7-5E6B81A697BB}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -13290,13 +12919,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -13304,10 +12933,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C2" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -13315,10 +12944,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C3" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -13326,10 +12955,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C4" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -13337,10 +12966,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C5" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -13348,10 +12977,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>272</v>
+      </c>
+      <c r="C6" t="s">
         <v>277</v>
-      </c>
-      <c r="C6" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -13359,10 +12988,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C7" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -13370,10 +12999,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C8" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -13381,10 +13010,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C9" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -13392,10 +13021,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C10" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -13403,10 +13032,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C11" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -13414,10 +13043,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C12" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -13425,10 +13054,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C13" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -13436,10 +13065,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C14" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -13447,10 +13076,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C15" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -13458,10 +13087,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C16" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -13469,10 +13098,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C17" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -13480,10 +13109,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C18" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -13491,10 +13120,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C19" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -13502,10 +13131,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C20" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -13513,10 +13142,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C21" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -13524,10 +13153,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C22" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -13535,10 +13164,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C23" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -13546,10 +13175,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C24" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -13557,10 +13186,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C25" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -13568,10 +13197,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C26" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -13579,10 +13208,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C27" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -13590,10 +13219,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C28" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -13601,10 +13230,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C29" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -13612,10 +13241,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C30" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -13623,10 +13252,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C31" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -13634,10 +13263,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C32" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -13645,10 +13274,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C33" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -13656,10 +13285,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C34" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -13667,10 +13296,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C35" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -13678,10 +13307,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C36" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -13689,10 +13318,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C37" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -13700,10 +13329,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C38" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -13711,10 +13340,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C39" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -13722,10 +13351,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C40" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -13733,10 +13362,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C41" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -13744,10 +13373,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C42" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -13755,10 +13384,10 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C43" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -13766,10 +13395,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C44" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -13777,10 +13406,10 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C45" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -13788,10 +13417,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C46" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
@@ -13799,10 +13428,10 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C47" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
@@ -13810,10 +13439,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C48" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>

</xml_diff>